<commit_message>
short display names on variables
</commit_message>
<xml_diff>
--- a/spec/files/0_3_3_short_names.xlsx
+++ b/spec/files/0_3_3_short_names.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="4060" windowWidth="28800" windowHeight="16840" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="51200" yWindow="4060" windowWidth="28800" windowHeight="16840" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$47:$M$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$7</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="831">
   <si>
     <t>type</t>
   </si>
@@ -2516,6 +2516,24 @@
   </si>
   <si>
     <t>Uhrs</t>
+  </si>
+  <si>
+    <t>Parameter Short Display Name</t>
+  </si>
+  <si>
+    <t>Shorter Display Name</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>ExampleMeasure</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>blah blah</t>
   </si>
 </sst>
 </file>
@@ -2652,8 +2670,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1747">
+  <cellStyleXfs count="1761">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4517,7 +4549,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1747">
+  <cellStyles count="1761">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5391,6 +5423,13 @@
     <cellStyle name="Followed Hyperlink" xfId="1742" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1744" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1760" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6264,6 +6303,13 @@
     <cellStyle name="Hyperlink" xfId="1741" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1743" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1759" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7117,11 +7163,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA80"/>
+  <dimension ref="A1:AB80"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7130,28 +7176,28 @@
     <col min="2" max="2" width="47" style="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="30" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="30" customWidth="1"/>
-    <col min="13" max="14" width="7.83203125" style="30" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="30"/>
-    <col min="16" max="16" width="11.5" style="30" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="46.1640625" style="30" customWidth="1"/>
-    <col min="20" max="22" width="11.5" style="30"/>
-    <col min="23" max="23" width="13.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="11.5" style="30"/>
-    <col min="27" max="27" width="15.1640625" style="30" customWidth="1"/>
-    <col min="28" max="16384" width="11.5" style="30"/>
+    <col min="5" max="6" width="24.1640625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="30" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" style="30" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="30" customWidth="1"/>
+    <col min="14" max="15" width="7.83203125" style="30" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="30"/>
+    <col min="17" max="17" width="11.5" style="30" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="46.1640625" style="30" customWidth="1"/>
+    <col min="21" max="23" width="11.5" style="30"/>
+    <col min="24" max="24" width="13.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="11.5" style="30"/>
+    <col min="28" max="28" width="15.1640625" style="30" customWidth="1"/>
+    <col min="29" max="16384" width="11.5" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18">
+    <row r="1" spans="1:28" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7161,32 +7207,33 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="20" t="s">
         <v>475</v>
       </c>
-      <c r="K1" s="21"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="21"/>
+      <c r="P1" s="36" t="s">
         <v>476</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="46"/>
+      <c r="Q1" s="22"/>
       <c r="R1" s="46"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="55" t="s">
+      <c r="S1" s="46"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="55"/>
       <c r="V1" s="55"/>
       <c r="W1" s="55"/>
       <c r="X1" s="55"/>
       <c r="Y1" s="55"/>
-    </row>
-    <row r="2" spans="1:27" s="8" customFormat="1" ht="15">
+      <c r="Z1" s="55"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7199,12 +7246,12 @@
       <c r="D2" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="Q2" s="47"/>
+      <c r="J2" s="9"/>
       <c r="R2" s="47"/>
-    </row>
-    <row r="3" spans="1:27" s="51" customFormat="1" ht="45">
+      <c r="S2" s="47"/>
+    </row>
+    <row r="3" spans="1:28" s="51" customFormat="1" ht="45">
       <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
@@ -7221,67 +7268,70 @@
         <v>36</v>
       </c>
       <c r="F3" s="52" t="s">
+        <v>825</v>
+      </c>
+      <c r="G3" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="H3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="I3" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="J3" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="K3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="L3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="M3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="52" t="s">
+      <c r="N3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="52" t="s">
+      <c r="O3" s="52" t="s">
         <v>621</v>
       </c>
-      <c r="O3" s="52" t="s">
+      <c r="P3" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="P3" s="52" t="s">
+      <c r="Q3" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="R3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="52" t="s">
+      <c r="S3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="52" t="s">
+      <c r="T3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="U3" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="V3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="51" t="s">
+      <c r="W3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="51" t="s">
+      <c r="X3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="51" t="s">
+      <c r="Y3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="51" t="s">
+      <c r="AB3" s="51" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="40" customFormat="1">
+    <row r="4" spans="1:28" s="40" customFormat="1">
       <c r="A4" s="40" t="b">
         <v>1</v>
       </c>
@@ -7297,12 +7347,12 @@
       <c r="E4" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="41"/>
       <c r="J4" s="41"/>
-      <c r="Q4" s="48"/>
+      <c r="K4" s="41"/>
       <c r="R4" s="48"/>
-    </row>
-    <row r="5" spans="1:27" s="42" customFormat="1">
+      <c r="S4" s="48"/>
+    </row>
+    <row r="5" spans="1:28" s="42" customFormat="1">
       <c r="A5" s="45"/>
       <c r="B5" s="45" t="s">
         <v>22</v>
@@ -7315,52 +7365,58 @@
         <v>76</v>
       </c>
       <c r="F5" s="45" t="s">
+        <v>826</v>
+      </c>
+      <c r="G5" s="45" t="s">
         <v>623</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="H5" s="45" t="s">
         <v>643</v>
       </c>
-      <c r="H5" s="45">
-        <v>0</v>
-      </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43">
-        <v>0</v>
-      </c>
-      <c r="K5" s="42">
+      <c r="I5" s="45">
+        <v>0</v>
+      </c>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43">
+        <v>0</v>
+      </c>
+      <c r="L5" s="42">
         <v>359</v>
       </c>
-      <c r="L5" s="42">
+      <c r="M5" s="42">
         <v>180</v>
       </c>
-      <c r="M5" s="44">
-        <f t="shared" ref="M5" si="0">(K5-J5)/6</f>
+      <c r="N5" s="44">
+        <f t="shared" ref="N5" si="0">(L5-K5)/6</f>
         <v>59.833333333333336</v>
       </c>
-      <c r="Q5" s="44" t="s">
+      <c r="R5" s="44" t="s">
         <v>626</v>
       </c>
-      <c r="R5" s="44"/>
-    </row>
-    <row r="6" spans="1:27" s="37" customFormat="1">
+      <c r="S5" s="44"/>
+    </row>
+    <row r="6" spans="1:28" s="37" customFormat="1">
       <c r="A6" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>640</v>
       </c>
+      <c r="C6" s="37" t="s">
+        <v>828</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>641</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="H6" s="38"/>
       <c r="I6" s="38"/>
-      <c r="Q6" s="49"/>
+      <c r="J6" s="38"/>
       <c r="R6" s="49"/>
-    </row>
-    <row r="7" spans="1:27">
+      <c r="S6" s="49"/>
+    </row>
+    <row r="7" spans="1:28">
       <c r="B7" s="30" t="s">
         <v>21</v>
       </c>
@@ -7370,311 +7426,319 @@
       <c r="E7" s="30" t="s">
         <v>642</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="J7" s="3"/>
+      <c r="F7" s="30" t="s">
+        <v>827</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>829</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>830</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="Q7" s="50"/>
-    </row>
-    <row r="8" spans="1:27">
-      <c r="H8" s="30"/>
+      <c r="P7" s="3"/>
+      <c r="R7" s="50"/>
+    </row>
+    <row r="8" spans="1:28">
       <c r="I8" s="30"/>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="H9" s="30"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:28">
       <c r="I9" s="30"/>
-    </row>
-    <row r="10" spans="1:27">
-      <c r="H10" s="30"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:28">
       <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="1:27">
-      <c r="H11" s="30"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:28">
       <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:27">
-      <c r="H12" s="30"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:28">
       <c r="I12" s="30"/>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="H13" s="30"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="1:28">
       <c r="I13" s="30"/>
-    </row>
-    <row r="14" spans="1:27">
-      <c r="H14" s="30"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:28">
       <c r="I14" s="30"/>
-    </row>
-    <row r="15" spans="1:27">
-      <c r="H15" s="30"/>
+      <c r="J14" s="30"/>
+    </row>
+    <row r="15" spans="1:28">
       <c r="I15" s="30"/>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="H16" s="30"/>
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="1:28">
       <c r="I16" s="30"/>
-    </row>
-    <row r="17" spans="8:9">
-      <c r="H17" s="30"/>
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" spans="9:10">
       <c r="I17" s="30"/>
-    </row>
-    <row r="18" spans="8:9">
-      <c r="H18" s="30"/>
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" spans="9:10">
       <c r="I18" s="30"/>
-    </row>
-    <row r="19" spans="8:9">
-      <c r="H19" s="30"/>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" spans="9:10">
       <c r="I19" s="30"/>
-    </row>
-    <row r="20" spans="8:9">
-      <c r="H20" s="30"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="9:10">
       <c r="I20" s="30"/>
-    </row>
-    <row r="21" spans="8:9">
-      <c r="H21" s="30"/>
+      <c r="J20" s="30"/>
+    </row>
+    <row r="21" spans="9:10">
       <c r="I21" s="30"/>
-    </row>
-    <row r="22" spans="8:9">
-      <c r="H22" s="30"/>
+      <c r="J21" s="30"/>
+    </row>
+    <row r="22" spans="9:10">
       <c r="I22" s="30"/>
-    </row>
-    <row r="23" spans="8:9">
-      <c r="H23" s="30"/>
+      <c r="J22" s="30"/>
+    </row>
+    <row r="23" spans="9:10">
       <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="8:9">
-      <c r="H24" s="30"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="9:10">
       <c r="I24" s="30"/>
-    </row>
-    <row r="25" spans="8:9">
-      <c r="H25" s="30"/>
+      <c r="J24" s="30"/>
+    </row>
+    <row r="25" spans="9:10">
       <c r="I25" s="30"/>
-    </row>
-    <row r="26" spans="8:9">
-      <c r="H26" s="30"/>
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" spans="9:10">
       <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="8:9">
-      <c r="H27" s="30"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="9:10">
       <c r="I27" s="30"/>
-    </row>
-    <row r="28" spans="8:9">
-      <c r="H28" s="30"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="9:10">
       <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="8:9">
-      <c r="H29" s="30"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="9:10">
       <c r="I29" s="30"/>
-    </row>
-    <row r="30" spans="8:9">
-      <c r="H30" s="30"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="9:10">
       <c r="I30" s="30"/>
-    </row>
-    <row r="31" spans="8:9">
-      <c r="H31" s="30"/>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="9:10">
       <c r="I31" s="30"/>
-    </row>
-    <row r="32" spans="8:9">
-      <c r="H32" s="30"/>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" spans="9:10">
       <c r="I32" s="30"/>
-    </row>
-    <row r="33" spans="8:9">
-      <c r="H33" s="30"/>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="9:10">
       <c r="I33" s="30"/>
-    </row>
-    <row r="34" spans="8:9">
-      <c r="H34" s="30"/>
+      <c r="J33" s="30"/>
+    </row>
+    <row r="34" spans="9:10">
       <c r="I34" s="30"/>
-    </row>
-    <row r="35" spans="8:9">
-      <c r="H35" s="30"/>
+      <c r="J34" s="30"/>
+    </row>
+    <row r="35" spans="9:10">
       <c r="I35" s="30"/>
-    </row>
-    <row r="36" spans="8:9">
-      <c r="H36" s="30"/>
+      <c r="J35" s="30"/>
+    </row>
+    <row r="36" spans="9:10">
       <c r="I36" s="30"/>
-    </row>
-    <row r="37" spans="8:9">
-      <c r="H37" s="30"/>
+      <c r="J36" s="30"/>
+    </row>
+    <row r="37" spans="9:10">
       <c r="I37" s="30"/>
-    </row>
-    <row r="38" spans="8:9">
-      <c r="H38" s="30"/>
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38" spans="9:10">
       <c r="I38" s="30"/>
-    </row>
-    <row r="39" spans="8:9">
-      <c r="H39" s="30"/>
+      <c r="J38" s="30"/>
+    </row>
+    <row r="39" spans="9:10">
       <c r="I39" s="30"/>
-    </row>
-    <row r="40" spans="8:9">
-      <c r="H40" s="30"/>
+      <c r="J39" s="30"/>
+    </row>
+    <row r="40" spans="9:10">
       <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="8:9">
-      <c r="H41" s="30"/>
+      <c r="J40" s="30"/>
+    </row>
+    <row r="41" spans="9:10">
       <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="8:9">
-      <c r="H42" s="30"/>
+      <c r="J41" s="30"/>
+    </row>
+    <row r="42" spans="9:10">
       <c r="I42" s="30"/>
-    </row>
-    <row r="43" spans="8:9">
-      <c r="H43" s="30"/>
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" spans="9:10">
       <c r="I43" s="30"/>
-    </row>
-    <row r="44" spans="8:9">
-      <c r="H44" s="30"/>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="9:10">
       <c r="I44" s="30"/>
-    </row>
-    <row r="45" spans="8:9">
-      <c r="H45" s="30"/>
+      <c r="J44" s="30"/>
+    </row>
+    <row r="45" spans="9:10">
       <c r="I45" s="30"/>
-    </row>
-    <row r="46" spans="8:9">
-      <c r="H46" s="30"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46" spans="9:10">
       <c r="I46" s="30"/>
-    </row>
-    <row r="47" spans="8:9">
-      <c r="H47" s="30"/>
+      <c r="J46" s="30"/>
+    </row>
+    <row r="47" spans="9:10">
       <c r="I47" s="30"/>
-    </row>
-    <row r="48" spans="8:9">
-      <c r="H48" s="30"/>
+      <c r="J47" s="30"/>
+    </row>
+    <row r="48" spans="9:10">
       <c r="I48" s="30"/>
-    </row>
-    <row r="49" spans="8:9">
-      <c r="H49" s="30"/>
+      <c r="J48" s="30"/>
+    </row>
+    <row r="49" spans="9:10">
       <c r="I49" s="30"/>
-    </row>
-    <row r="50" spans="8:9">
-      <c r="H50" s="30"/>
+      <c r="J49" s="30"/>
+    </row>
+    <row r="50" spans="9:10">
       <c r="I50" s="30"/>
-    </row>
-    <row r="51" spans="8:9">
-      <c r="H51" s="30"/>
+      <c r="J50" s="30"/>
+    </row>
+    <row r="51" spans="9:10">
       <c r="I51" s="30"/>
-    </row>
-    <row r="52" spans="8:9">
-      <c r="H52" s="30"/>
+      <c r="J51" s="30"/>
+    </row>
+    <row r="52" spans="9:10">
       <c r="I52" s="30"/>
-    </row>
-    <row r="53" spans="8:9">
-      <c r="H53" s="30"/>
+      <c r="J52" s="30"/>
+    </row>
+    <row r="53" spans="9:10">
       <c r="I53" s="30"/>
-    </row>
-    <row r="54" spans="8:9">
-      <c r="H54" s="30"/>
+      <c r="J53" s="30"/>
+    </row>
+    <row r="54" spans="9:10">
       <c r="I54" s="30"/>
-    </row>
-    <row r="55" spans="8:9">
-      <c r="H55" s="30"/>
+      <c r="J54" s="30"/>
+    </row>
+    <row r="55" spans="9:10">
       <c r="I55" s="30"/>
-    </row>
-    <row r="56" spans="8:9">
-      <c r="H56" s="30"/>
+      <c r="J55" s="30"/>
+    </row>
+    <row r="56" spans="9:10">
       <c r="I56" s="30"/>
-    </row>
-    <row r="57" spans="8:9">
-      <c r="H57" s="30"/>
+      <c r="J56" s="30"/>
+    </row>
+    <row r="57" spans="9:10">
       <c r="I57" s="30"/>
-    </row>
-    <row r="58" spans="8:9">
-      <c r="H58" s="30"/>
+      <c r="J57" s="30"/>
+    </row>
+    <row r="58" spans="9:10">
       <c r="I58" s="30"/>
-    </row>
-    <row r="59" spans="8:9">
-      <c r="H59" s="30"/>
+      <c r="J58" s="30"/>
+    </row>
+    <row r="59" spans="9:10">
       <c r="I59" s="30"/>
-    </row>
-    <row r="60" spans="8:9">
-      <c r="H60" s="30"/>
+      <c r="J59" s="30"/>
+    </row>
+    <row r="60" spans="9:10">
       <c r="I60" s="30"/>
-    </row>
-    <row r="61" spans="8:9">
-      <c r="H61" s="30"/>
+      <c r="J60" s="30"/>
+    </row>
+    <row r="61" spans="9:10">
       <c r="I61" s="30"/>
-    </row>
-    <row r="62" spans="8:9">
-      <c r="H62" s="30"/>
+      <c r="J61" s="30"/>
+    </row>
+    <row r="62" spans="9:10">
       <c r="I62" s="30"/>
-    </row>
-    <row r="63" spans="8:9">
-      <c r="H63" s="30"/>
+      <c r="J62" s="30"/>
+    </row>
+    <row r="63" spans="9:10">
       <c r="I63" s="30"/>
-    </row>
-    <row r="64" spans="8:9">
-      <c r="H64" s="30"/>
+      <c r="J63" s="30"/>
+    </row>
+    <row r="64" spans="9:10">
       <c r="I64" s="30"/>
-    </row>
-    <row r="65" spans="8:9">
-      <c r="H65" s="30"/>
+      <c r="J64" s="30"/>
+    </row>
+    <row r="65" spans="9:10">
       <c r="I65" s="30"/>
-    </row>
-    <row r="66" spans="8:9">
-      <c r="H66" s="30"/>
+      <c r="J65" s="30"/>
+    </row>
+    <row r="66" spans="9:10">
       <c r="I66" s="30"/>
-    </row>
-    <row r="67" spans="8:9">
-      <c r="H67" s="30"/>
+      <c r="J66" s="30"/>
+    </row>
+    <row r="67" spans="9:10">
       <c r="I67" s="30"/>
-    </row>
-    <row r="68" spans="8:9">
-      <c r="H68" s="30"/>
+      <c r="J67" s="30"/>
+    </row>
+    <row r="68" spans="9:10">
       <c r="I68" s="30"/>
-    </row>
-    <row r="69" spans="8:9">
-      <c r="H69" s="30"/>
+      <c r="J68" s="30"/>
+    </row>
+    <row r="69" spans="9:10">
       <c r="I69" s="30"/>
-    </row>
-    <row r="70" spans="8:9">
-      <c r="H70" s="30"/>
+      <c r="J69" s="30"/>
+    </row>
+    <row r="70" spans="9:10">
       <c r="I70" s="30"/>
-    </row>
-    <row r="71" spans="8:9">
-      <c r="H71" s="30"/>
+      <c r="J70" s="30"/>
+    </row>
+    <row r="71" spans="9:10">
       <c r="I71" s="30"/>
-    </row>
-    <row r="72" spans="8:9">
-      <c r="H72" s="30"/>
+      <c r="J71" s="30"/>
+    </row>
+    <row r="72" spans="9:10">
       <c r="I72" s="30"/>
-    </row>
-    <row r="73" spans="8:9">
-      <c r="H73" s="30"/>
+      <c r="J72" s="30"/>
+    </row>
+    <row r="73" spans="9:10">
       <c r="I73" s="30"/>
-    </row>
-    <row r="74" spans="8:9">
-      <c r="H74" s="30"/>
+      <c r="J73" s="30"/>
+    </row>
+    <row r="74" spans="9:10">
       <c r="I74" s="30"/>
-    </row>
-    <row r="75" spans="8:9">
-      <c r="H75" s="30"/>
+      <c r="J74" s="30"/>
+    </row>
+    <row r="75" spans="9:10">
       <c r="I75" s="30"/>
-    </row>
-    <row r="76" spans="8:9">
-      <c r="H76" s="30"/>
+      <c r="J75" s="30"/>
+    </row>
+    <row r="76" spans="9:10">
       <c r="I76" s="30"/>
-    </row>
-    <row r="77" spans="8:9">
-      <c r="H77" s="30"/>
+      <c r="J76" s="30"/>
+    </row>
+    <row r="77" spans="9:10">
       <c r="I77" s="30"/>
-    </row>
-    <row r="78" spans="8:9">
-      <c r="H78" s="30"/>
+      <c r="J77" s="30"/>
+    </row>
+    <row r="78" spans="9:10">
       <c r="I78" s="30"/>
-    </row>
-    <row r="79" spans="8:9">
-      <c r="H79" s="30"/>
+      <c r="J78" s="30"/>
+    </row>
+    <row r="79" spans="9:10">
       <c r="I79" s="30"/>
-    </row>
-    <row r="80" spans="8:9">
-      <c r="H80" s="30"/>
+      <c r="J79" s="30"/>
+    </row>
+    <row r="80" spans="9:10">
       <c r="I80" s="30"/>
+      <c r="J80" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Z7"/>
+  <autoFilter ref="A2:AA7"/>
   <mergeCells count="1">
-    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="U1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7690,9 +7754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>